<commit_message>
Add result for New York
</commit_message>
<xml_diff>
--- a/data/改进策略结果.xlsx
+++ b/data/改进策略结果.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wangyw15\Desktop\2023E\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34E06709-B750-4D78-95FF-F4E0B76E26B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC46B39-A1A1-42DA-9A48-4FB4B3504DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1250" windowWidth="21300" windowHeight="12430" xr2:uid="{28A72D09-0D8D-45BE-8D0A-CBCC4F2108E1}"/>
   </bookViews>
@@ -36,13 +36,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>from</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>California</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New York</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,28 +419,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32E3874-F50C-4777-A525-DF28BD7C5906}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>0.59146234117887098</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.58022721879154404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.69032135242221404</v>
+      </c>
+      <c r="C3">
+        <v>0.68075655255527501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>